<commit_message>
reshaped, fixed geo_cw, todo: merge fields
</commit_message>
<xml_diff>
--- a/KEN_IHBS_2016.xlsx
+++ b/KEN_IHBS_2016.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tim/Documents/GitHub/Kenya_2018/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8889995D-4852-F341-8688-2CE6295F47C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="135" windowWidth="12435" windowHeight="10800"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Food_poverty" sheetId="1" r:id="rId1"/>
@@ -16,12 +22,12 @@
     <sheet name="Food_poverty_children" sheetId="7" r:id="rId7"/>
     <sheet name="geo_cw" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="207">
   <si>
     <t>Mombasa</t>
   </si>
@@ -647,12 +653,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="168" formatCode="###0.0;###0.0"/>
-    <numFmt numFmtId="169" formatCode="#,##0;#,##0"/>
-    <numFmt numFmtId="170" formatCode="###0;###0"/>
-    <numFmt numFmtId="175" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="###0.0;###0.0"/>
+    <numFmt numFmtId="165" formatCode="#,##0;#,##0"/>
+    <numFmt numFmtId="166" formatCode="###0;###0"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
   <fonts count="23" x14ac:knownFonts="1">
     <font>
@@ -1176,26 +1182,26 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1204,13 +1210,13 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="175" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1219,13 +1225,13 @@
     <xf numFmtId="1" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1235,10 +1241,10 @@
     <xf numFmtId="1" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="175" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1298,6 +1304,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1345,7 +1354,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1378,9 +1387,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1413,6 +1439,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1588,27 +1631,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A14" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="4"/>
-    <col min="3" max="3" width="21.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="4"/>
+    <col min="3" max="3" width="21.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="4"/>
+    <col min="7" max="7" width="8.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.1640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>47</v>
       </c>
@@ -1634,7 +1677,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="str">
         <f>VLOOKUP(B2,geo_cw!A$2:H$49,2)</f>
         <v>Mombasa</v>
@@ -1661,7 +1704,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="str">
         <f>VLOOKUP(B3,geo_cw!A$2:H$49,2)</f>
         <v>Kwale</v>
@@ -1688,7 +1731,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="str">
         <f>VLOOKUP(B4,geo_cw!A$2:H$49,2)</f>
         <v>Kilifi</v>
@@ -1715,7 +1758,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="str">
         <f>VLOOKUP(B5,geo_cw!A$2:H$49,2)</f>
         <v>Tana River</v>
@@ -1742,7 +1785,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="str">
         <f>VLOOKUP(B6,geo_cw!A$2:H$49,2)</f>
         <v>Lamu</v>
@@ -1769,7 +1812,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="str">
         <f>VLOOKUP(B7,geo_cw!A$2:H$49,2)</f>
         <v>Taita Taveta</v>
@@ -1796,7 +1839,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="str">
         <f>VLOOKUP(B8,geo_cw!A$2:H$49,2)</f>
         <v>Garissa</v>
@@ -1823,7 +1866,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="str">
         <f>VLOOKUP(B9,geo_cw!A$2:H$49,2)</f>
         <v>Wajir</v>
@@ -1850,7 +1893,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="str">
         <f>VLOOKUP(B10,geo_cw!A$2:H$49,2)</f>
         <v>Mandera</v>
@@ -1877,7 +1920,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="str">
         <f>VLOOKUP(B11,geo_cw!A$2:H$49,2)</f>
         <v>Marsabit</v>
@@ -1904,7 +1947,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="str">
         <f>VLOOKUP(B12,geo_cw!A$2:H$49,2)</f>
         <v>Isiolo</v>
@@ -1931,7 +1974,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="str">
         <f>VLOOKUP(B13,geo_cw!A$2:H$49,2)</f>
         <v>Meru</v>
@@ -1958,7 +2001,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="str">
         <f>VLOOKUP(B14,geo_cw!A$2:H$49,2)</f>
         <v>Tharaka-Nithi</v>
@@ -1985,7 +2028,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="str">
         <f>VLOOKUP(B15,geo_cw!A$2:H$49,2)</f>
         <v>Embu</v>
@@ -2012,7 +2055,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="str">
         <f>VLOOKUP(B16,geo_cw!A$2:H$49,2)</f>
         <v>Kitui</v>
@@ -2039,7 +2082,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="str">
         <f>VLOOKUP(B17,geo_cw!A$2:H$49,2)</f>
         <v>Machakos</v>
@@ -2066,7 +2109,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="str">
         <f>VLOOKUP(B18,geo_cw!A$2:H$49,2)</f>
         <v>Makueni</v>
@@ -2093,7 +2136,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="str">
         <f>VLOOKUP(B19,geo_cw!A$2:H$49,2)</f>
         <v>Nyandarua</v>
@@ -2120,7 +2163,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="str">
         <f>VLOOKUP(B20,geo_cw!A$2:H$49,2)</f>
         <v>Nyeri</v>
@@ -2147,7 +2190,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="str">
         <f>VLOOKUP(B21,geo_cw!A$2:H$49,2)</f>
         <v>Kirinyaga</v>
@@ -2174,10 +2217,10 @@
         <v>114</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="str">
         <f>VLOOKUP(B22,geo_cw!A$2:H$49,2)</f>
-        <v>Mombasa</v>
+        <v>Murang'a</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>20</v>
@@ -2201,7 +2244,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="str">
         <f>VLOOKUP(B23,geo_cw!A$2:H$49,2)</f>
         <v>Kiambu</v>
@@ -2228,7 +2271,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="str">
         <f>VLOOKUP(B24,geo_cw!A$2:H$49,2)</f>
         <v>Turkana</v>
@@ -2255,7 +2298,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="str">
         <f>VLOOKUP(B25,geo_cw!A$2:H$49,2)</f>
         <v>West Pokot</v>
@@ -2282,7 +2325,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="str">
         <f>VLOOKUP(B26,geo_cw!A$2:H$49,2)</f>
         <v>Samburu</v>
@@ -2309,7 +2352,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="str">
         <f>VLOOKUP(B27,geo_cw!A$2:H$49,2)</f>
         <v>Trans Nzoia</v>
@@ -2336,7 +2379,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="str">
         <f>VLOOKUP(B28,geo_cw!A$2:H$49,2)</f>
         <v>Uasin Gishu</v>
@@ -2363,10 +2406,9 @@
         <v>433</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="str">
-        <f>VLOOKUP(B29,geo_cw!A$2:H$49,2)</f>
-        <v>Busia</v>
+    <row r="29" spans="1:8" ht="24" x14ac:dyDescent="0.15">
+      <c r="A29" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>27</v>
@@ -2390,7 +2432,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="str">
         <f>VLOOKUP(B30,geo_cw!A$2:H$49,2)</f>
         <v>Nandi</v>
@@ -2417,7 +2459,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="str">
         <f>VLOOKUP(B31,geo_cw!A$2:H$49,2)</f>
         <v>Baringo</v>
@@ -2444,7 +2486,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="str">
         <f>VLOOKUP(B32,geo_cw!A$2:H$49,2)</f>
         <v>Laikipia</v>
@@ -2471,7 +2513,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="str">
         <f>VLOOKUP(B33,geo_cw!A$2:H$49,2)</f>
         <v>Nakuru</v>
@@ -2498,7 +2540,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="str">
         <f>VLOOKUP(B34,geo_cw!A$2:H$49,2)</f>
         <v>Narok</v>
@@ -2525,7 +2567,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A35" s="4" t="str">
         <f>VLOOKUP(B35,geo_cw!A$2:H$49,2)</f>
         <v>Kajiado</v>
@@ -2552,7 +2594,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A36" s="4" t="str">
         <f>VLOOKUP(B36,geo_cw!A$2:H$49,2)</f>
         <v>Kericho</v>
@@ -2579,7 +2621,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="str">
         <f>VLOOKUP(B37,geo_cw!A$2:H$49,2)</f>
         <v>Bomet</v>
@@ -2606,7 +2648,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="str">
         <f>VLOOKUP(B38,geo_cw!A$2:H$49,2)</f>
         <v>Kakamega</v>
@@ -2633,7 +2675,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="str">
         <f>VLOOKUP(B39,geo_cw!A$2:H$49,2)</f>
         <v>Vihiga</v>
@@ -2660,7 +2702,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="str">
         <f>VLOOKUP(B40,geo_cw!A$2:H$49,2)</f>
         <v>Bungoma</v>
@@ -2687,7 +2729,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A41" s="4" t="str">
         <f>VLOOKUP(B41,geo_cw!A$2:H$49,2)</f>
         <v>Busia</v>
@@ -2714,7 +2756,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A42" s="4" t="str">
         <f>VLOOKUP(B42,geo_cw!A$2:H$49,2)</f>
         <v>Siaya</v>
@@ -2741,7 +2783,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A43" s="4" t="str">
         <f>VLOOKUP(B43,geo_cw!A$2:H$49,2)</f>
         <v>Kisumu</v>
@@ -2768,7 +2810,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A44" s="4" t="str">
         <f>VLOOKUP(B44,geo_cw!A$2:H$49,2)</f>
         <v>Homa Bay</v>
@@ -2795,7 +2837,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A45" s="4" t="str">
         <f>VLOOKUP(B45,geo_cw!A$2:H$49,2)</f>
         <v>Migori</v>
@@ -2822,7 +2864,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A46" s="4" t="str">
         <f>VLOOKUP(B46,geo_cw!A$2:H$49,2)</f>
         <v>Kisii</v>
@@ -2849,7 +2891,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A47" s="4" t="str">
         <f>VLOOKUP(B47,geo_cw!A$2:H$49,2)</f>
         <v>Nyamira</v>
@@ -2876,7 +2918,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A48" s="4" t="str">
         <f>VLOOKUP(B48,geo_cw!A$2:H$49,2)</f>
         <v>Nairobi</v>
@@ -2903,7 +2945,10 @@
         <v>717</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A49" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="B49" s="4" t="s">
         <v>84</v>
       </c>
@@ -2932,27 +2977,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="4"/>
+    <col min="3" max="3" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.1640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
         <v>47</v>
       </c>
@@ -2978,7 +3023,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="str">
         <f>VLOOKUP(B2,geo_cw!A$2:H$49,2)</f>
         <v>Mombasa</v>
@@ -3005,7 +3050,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="str">
         <f>VLOOKUP(B3,geo_cw!A$2:H$49,2)</f>
         <v>Kwale</v>
@@ -3032,7 +3077,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="str">
         <f>VLOOKUP(B4,geo_cw!A$2:H$49,2)</f>
         <v>Kilifi</v>
@@ -3059,7 +3104,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="str">
         <f>VLOOKUP(B5,geo_cw!A$2:H$49,2)</f>
         <v>Tana River</v>
@@ -3086,7 +3131,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="str">
         <f>VLOOKUP(B6,geo_cw!A$2:H$49,2)</f>
         <v>Lamu</v>
@@ -3113,7 +3158,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="str">
         <f>VLOOKUP(B7,geo_cw!A$2:H$49,2)</f>
         <v>Taita Taveta</v>
@@ -3140,7 +3185,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="str">
         <f>VLOOKUP(B8,geo_cw!A$2:H$49,2)</f>
         <v>Garissa</v>
@@ -3167,7 +3212,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="str">
         <f>VLOOKUP(B9,geo_cw!A$2:H$49,2)</f>
         <v>Wajir</v>
@@ -3194,7 +3239,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="str">
         <f>VLOOKUP(B10,geo_cw!A$2:H$49,2)</f>
         <v>Mandera</v>
@@ -3221,7 +3266,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="str">
         <f>VLOOKUP(B11,geo_cw!A$2:H$49,2)</f>
         <v>Marsabit</v>
@@ -3248,7 +3293,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="str">
         <f>VLOOKUP(B12,geo_cw!A$2:H$49,2)</f>
         <v>Isiolo</v>
@@ -3275,7 +3320,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="str">
         <f>VLOOKUP(B13,geo_cw!A$2:H$49,2)</f>
         <v>Meru</v>
@@ -3302,7 +3347,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="str">
         <f>VLOOKUP(B14,geo_cw!A$2:H$49,2)</f>
         <v>Tharaka-Nithi</v>
@@ -3329,7 +3374,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="str">
         <f>VLOOKUP(B15,geo_cw!A$2:H$49,2)</f>
         <v>Embu</v>
@@ -3356,7 +3401,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="str">
         <f>VLOOKUP(B16,geo_cw!A$2:H$49,2)</f>
         <v>Kitui</v>
@@ -3383,7 +3428,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="str">
         <f>VLOOKUP(B17,geo_cw!A$2:H$49,2)</f>
         <v>Machakos</v>
@@ -3410,7 +3455,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="str">
         <f>VLOOKUP(B18,geo_cw!A$2:H$49,2)</f>
         <v>Makueni</v>
@@ -3437,7 +3482,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="str">
         <f>VLOOKUP(B19,geo_cw!A$2:H$49,2)</f>
         <v>Nyandarua</v>
@@ -3464,7 +3509,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="str">
         <f>VLOOKUP(B20,geo_cw!A$2:H$49,2)</f>
         <v>Nyeri</v>
@@ -3491,7 +3536,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="str">
         <f>VLOOKUP(B21,geo_cw!A$2:H$49,2)</f>
         <v>Kirinyaga</v>
@@ -3518,10 +3563,10 @@
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="str">
         <f>VLOOKUP(B22,geo_cw!A$2:H$49,2)</f>
-        <v>Mombasa</v>
+        <v>Murang'a</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>20</v>
@@ -3545,7 +3590,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="str">
         <f>VLOOKUP(B23,geo_cw!A$2:H$49,2)</f>
         <v>Kiambu</v>
@@ -3572,7 +3617,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="str">
         <f>VLOOKUP(B24,geo_cw!A$2:H$49,2)</f>
         <v>Turkana</v>
@@ -3599,7 +3644,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="str">
         <f>VLOOKUP(B25,geo_cw!A$2:H$49,2)</f>
         <v>West Pokot</v>
@@ -3626,7 +3671,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="str">
         <f>VLOOKUP(B26,geo_cw!A$2:H$49,2)</f>
         <v>Samburu</v>
@@ -3653,7 +3698,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="str">
         <f>VLOOKUP(B27,geo_cw!A$2:H$49,2)</f>
         <v>Trans Nzoia</v>
@@ -3680,7 +3725,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="str">
         <f>VLOOKUP(B28,geo_cw!A$2:H$49,2)</f>
         <v>Uasin Gishu</v>
@@ -3707,10 +3752,9 @@
         <v>465</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="str">
-        <f>VLOOKUP(B29,geo_cw!A$2:H$49,2)</f>
-        <v>Busia</v>
+    <row r="29" spans="1:8" ht="24" x14ac:dyDescent="0.15">
+      <c r="A29" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>57</v>
@@ -3734,7 +3778,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="str">
         <f>VLOOKUP(B30,geo_cw!A$2:H$49,2)</f>
         <v>Nandi</v>
@@ -3761,7 +3805,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="str">
         <f>VLOOKUP(B31,geo_cw!A$2:H$49,2)</f>
         <v>Baringo</v>
@@ -3788,7 +3832,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="str">
         <f>VLOOKUP(B32,geo_cw!A$2:H$49,2)</f>
         <v>Laikipia</v>
@@ -3815,7 +3859,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="str">
         <f>VLOOKUP(B33,geo_cw!A$2:H$49,2)</f>
         <v>Nakuru</v>
@@ -3842,7 +3886,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="str">
         <f>VLOOKUP(B34,geo_cw!A$2:H$49,2)</f>
         <v>Narok</v>
@@ -3869,7 +3913,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A35" s="4" t="str">
         <f>VLOOKUP(B35,geo_cw!A$2:H$49,2)</f>
         <v>Kajiado</v>
@@ -3896,7 +3940,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A36" s="4" t="str">
         <f>VLOOKUP(B36,geo_cw!A$2:H$49,2)</f>
         <v>Kericho</v>
@@ -3923,7 +3967,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="str">
         <f>VLOOKUP(B37,geo_cw!A$2:H$49,2)</f>
         <v>Bomet</v>
@@ -3950,7 +3994,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="str">
         <f>VLOOKUP(B38,geo_cw!A$2:H$49,2)</f>
         <v>Kakamega</v>
@@ -3977,7 +4021,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="str">
         <f>VLOOKUP(B39,geo_cw!A$2:H$49,2)</f>
         <v>Vihiga</v>
@@ -4004,7 +4048,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="str">
         <f>VLOOKUP(B40,geo_cw!A$2:H$49,2)</f>
         <v>Bungoma</v>
@@ -4031,7 +4075,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A41" s="4" t="str">
         <f>VLOOKUP(B41,geo_cw!A$2:H$49,2)</f>
         <v>Busia</v>
@@ -4058,7 +4102,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A42" s="4" t="str">
         <f>VLOOKUP(B42,geo_cw!A$2:H$49,2)</f>
         <v>Siaya</v>
@@ -4085,7 +4129,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A43" s="4" t="str">
         <f>VLOOKUP(B43,geo_cw!A$2:H$49,2)</f>
         <v>Kisumu</v>
@@ -4112,7 +4156,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A44" s="4" t="str">
         <f>VLOOKUP(B44,geo_cw!A$2:H$49,2)</f>
         <v>Homa Bay</v>
@@ -4139,7 +4183,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A45" s="4" t="str">
         <f>VLOOKUP(B45,geo_cw!A$2:H$49,2)</f>
         <v>Migori</v>
@@ -4166,7 +4210,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A46" s="4" t="str">
         <f>VLOOKUP(B46,geo_cw!A$2:H$49,2)</f>
         <v>Kisii</v>
@@ -4193,7 +4237,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A47" s="4" t="str">
         <f>VLOOKUP(B47,geo_cw!A$2:H$49,2)</f>
         <v>Nyamira</v>
@@ -4220,7 +4264,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A48" s="4" t="str">
         <f>VLOOKUP(B48,geo_cw!A$2:H$49,2)</f>
         <v>Nairobi</v>
@@ -4247,7 +4291,10 @@
         <v>745</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A49" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="B49" s="4" t="s">
         <v>84</v>
       </c>
@@ -4276,27 +4323,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView topLeftCell="A22" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="4"/>
-    <col min="3" max="3" width="12.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="4"/>
+    <col min="3" max="3" width="12.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="4"/>
+    <col min="6" max="6" width="16.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.1640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
         <v>47</v>
       </c>
@@ -4322,7 +4369,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="str">
         <f>VLOOKUP(B2,geo_cw!A$2:H$49,2)</f>
         <v>Mombasa</v>
@@ -4349,7 +4396,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="str">
         <f>VLOOKUP(B3,geo_cw!A$2:H$49,2)</f>
         <v>Kwale</v>
@@ -4376,7 +4423,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="str">
         <f>VLOOKUP(B4,geo_cw!A$2:H$49,2)</f>
         <v>Kilifi</v>
@@ -4403,7 +4450,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="str">
         <f>VLOOKUP(B5,geo_cw!A$2:H$49,2)</f>
         <v>Tana River</v>
@@ -4430,7 +4477,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="str">
         <f>VLOOKUP(B6,geo_cw!A$2:H$49,2)</f>
         <v>Lamu</v>
@@ -4457,7 +4504,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="str">
         <f>VLOOKUP(B7,geo_cw!A$2:H$49,2)</f>
         <v>Taita Taveta</v>
@@ -4484,7 +4531,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="str">
         <f>VLOOKUP(B8,geo_cw!A$2:H$49,2)</f>
         <v>Garissa</v>
@@ -4511,7 +4558,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="str">
         <f>VLOOKUP(B9,geo_cw!A$2:H$49,2)</f>
         <v>Wajir</v>
@@ -4538,7 +4585,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="str">
         <f>VLOOKUP(B10,geo_cw!A$2:H$49,2)</f>
         <v>Mandera</v>
@@ -4565,7 +4612,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="str">
         <f>VLOOKUP(B11,geo_cw!A$2:H$49,2)</f>
         <v>Marsabit</v>
@@ -4592,7 +4639,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="str">
         <f>VLOOKUP(B12,geo_cw!A$2:H$49,2)</f>
         <v>Isiolo</v>
@@ -4619,7 +4666,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="str">
         <f>VLOOKUP(B13,geo_cw!A$2:H$49,2)</f>
         <v>Meru</v>
@@ -4646,7 +4693,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="24" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="str">
         <f>VLOOKUP(B14,geo_cw!A$2:H$49,2)</f>
         <v>Tharaka-Nithi</v>
@@ -4673,7 +4720,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="str">
         <f>VLOOKUP(B15,geo_cw!A$2:H$49,2)</f>
         <v>Embu</v>
@@ -4700,7 +4747,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="str">
         <f>VLOOKUP(B16,geo_cw!A$2:H$49,2)</f>
         <v>Kitui</v>
@@ -4727,7 +4774,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="str">
         <f>VLOOKUP(B17,geo_cw!A$2:H$49,2)</f>
         <v>Machakos</v>
@@ -4754,7 +4801,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="str">
         <f>VLOOKUP(B18,geo_cw!A$2:H$49,2)</f>
         <v>Makueni</v>
@@ -4781,7 +4828,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="str">
         <f>VLOOKUP(B19,geo_cw!A$2:H$49,2)</f>
         <v>Nyandarua</v>
@@ -4808,7 +4855,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="str">
         <f>VLOOKUP(B20,geo_cw!A$2:H$49,2)</f>
         <v>Nyeri</v>
@@ -4835,7 +4882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="str">
         <f>VLOOKUP(B21,geo_cw!A$2:H$49,2)</f>
         <v>Kirinyaga</v>
@@ -4862,7 +4909,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="str">
         <f>VLOOKUP(B22,geo_cw!A$2:H$49,2)</f>
         <v>Murang'a</v>
@@ -4889,7 +4936,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="str">
         <f>VLOOKUP(B23,geo_cw!A$2:H$49,2)</f>
         <v>Kiambu</v>
@@ -4916,7 +4963,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="str">
         <f>VLOOKUP(B24,geo_cw!A$2:H$49,2)</f>
         <v>Turkana</v>
@@ -4943,7 +4990,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="str">
         <f>VLOOKUP(B25,geo_cw!A$2:H$49,2)</f>
         <v>West Pokot</v>
@@ -4970,7 +5017,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="str">
         <f>VLOOKUP(B26,geo_cw!A$2:H$49,2)</f>
         <v>Samburu</v>
@@ -4997,7 +5044,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="str">
         <f>VLOOKUP(B27,geo_cw!A$2:H$49,2)</f>
         <v>Trans Nzoia</v>
@@ -5024,7 +5071,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="str">
         <f>VLOOKUP(B28,geo_cw!A$2:H$49,2)</f>
         <v>Uasin Gishu</v>
@@ -5051,10 +5098,9 @@
         <v>137</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="str">
-        <f>VLOOKUP(B29,geo_cw!A$2:H$49,2)</f>
-        <v>Busia</v>
+    <row r="29" spans="1:8" ht="24" x14ac:dyDescent="0.15">
+      <c r="A29" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>27</v>
@@ -5078,7 +5124,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="str">
         <f>VLOOKUP(B30,geo_cw!A$2:H$49,2)</f>
         <v>Nandi</v>
@@ -5105,7 +5151,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="str">
         <f>VLOOKUP(B31,geo_cw!A$2:H$49,2)</f>
         <v>Baringo</v>
@@ -5132,7 +5178,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="str">
         <f>VLOOKUP(B32,geo_cw!A$2:H$49,2)</f>
         <v>Laikipia</v>
@@ -5159,7 +5205,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="str">
         <f>VLOOKUP(B33,geo_cw!A$2:H$49,2)</f>
         <v>Nakuru</v>
@@ -5186,7 +5232,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="str">
         <f>VLOOKUP(B34,geo_cw!A$2:H$49,2)</f>
         <v>Narok</v>
@@ -5213,7 +5259,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A35" s="4" t="str">
         <f>VLOOKUP(B35,geo_cw!A$2:H$49,2)</f>
         <v>Kajiado</v>
@@ -5240,7 +5286,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A36" s="4" t="str">
         <f>VLOOKUP(B36,geo_cw!A$2:H$49,2)</f>
         <v>Kericho</v>
@@ -5267,7 +5313,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="str">
         <f>VLOOKUP(B37,geo_cw!A$2:H$49,2)</f>
         <v>Bomet</v>
@@ -5294,7 +5340,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="str">
         <f>VLOOKUP(B38,geo_cw!A$2:H$49,2)</f>
         <v>Kakamega</v>
@@ -5321,7 +5367,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="str">
         <f>VLOOKUP(B39,geo_cw!A$2:H$49,2)</f>
         <v>Vihiga</v>
@@ -5348,7 +5394,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="str">
         <f>VLOOKUP(B40,geo_cw!A$2:H$49,2)</f>
         <v>Bungoma</v>
@@ -5375,7 +5421,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A41" s="4" t="str">
         <f>VLOOKUP(B41,geo_cw!A$2:H$49,2)</f>
         <v>Busia</v>
@@ -5402,7 +5448,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A42" s="4" t="str">
         <f>VLOOKUP(B42,geo_cw!A$2:H$49,2)</f>
         <v>Siaya</v>
@@ -5429,7 +5475,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A43" s="4" t="str">
         <f>VLOOKUP(B43,geo_cw!A$2:H$49,2)</f>
         <v>Kisumu</v>
@@ -5456,7 +5502,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A44" s="4" t="str">
         <f>VLOOKUP(B44,geo_cw!A$2:H$49,2)</f>
         <v>Homa Bay</v>
@@ -5483,7 +5529,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A45" s="4" t="str">
         <f>VLOOKUP(B45,geo_cw!A$2:H$49,2)</f>
         <v>Migori</v>
@@ -5510,7 +5556,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A46" s="4" t="str">
         <f>VLOOKUP(B46,geo_cw!A$2:H$49,2)</f>
         <v>Kisii</v>
@@ -5537,7 +5583,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A47" s="4" t="str">
         <f>VLOOKUP(B47,geo_cw!A$2:H$49,2)</f>
         <v>Nyamira</v>
@@ -5564,7 +5610,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A48" s="4" t="str">
         <f>VLOOKUP(B48,geo_cw!A$2:H$49,2)</f>
         <v>Nairobi</v>
@@ -5591,7 +5637,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A49" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="B49" s="4" t="s">
         <v>84</v>
       </c>
@@ -5620,22 +5669,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="7.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.1640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>75</v>
       </c>
@@ -5646,7 +5695,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>72</v>
       </c>
@@ -5662,7 +5711,7 @@
       <c r="G2" s="20"/>
       <c r="H2" s="17"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>63</v>
       </c>
@@ -5678,7 +5727,7 @@
       <c r="G3" s="20"/>
       <c r="H3" s="17"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>64</v>
       </c>
@@ -5694,7 +5743,7 @@
       <c r="G4" s="20"/>
       <c r="H4" s="17"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
         <v>65</v>
       </c>
@@ -5710,7 +5759,7 @@
       <c r="G5" s="20"/>
       <c r="H5" s="17"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
         <v>66</v>
       </c>
@@ -5726,7 +5775,7 @@
       <c r="G6" s="20"/>
       <c r="H6" s="17"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A7" s="5" t="s">
         <v>67</v>
       </c>
@@ -5742,7 +5791,7 @@
       <c r="G7" s="20"/>
       <c r="H7" s="17"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
         <v>68</v>
       </c>
@@ -5758,7 +5807,7 @@
       <c r="G8" s="20"/>
       <c r="H8" s="17"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A9" s="5" t="s">
         <v>69</v>
       </c>
@@ -5774,7 +5823,7 @@
       <c r="G9" s="20"/>
       <c r="H9" s="17"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A10" s="5" t="s">
         <v>70</v>
       </c>
@@ -5786,7 +5835,7 @@
       <c r="G10" s="20"/>
       <c r="H10" s="17"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="s">
         <v>71</v>
       </c>
@@ -5802,7 +5851,7 @@
       <c r="G11" s="20"/>
       <c r="H11" s="17"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A12" s="5" t="s">
         <v>72</v>
       </c>
@@ -5818,7 +5867,7 @@
       <c r="G12" s="20"/>
       <c r="H12" s="17"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A13" s="5" t="s">
         <v>63</v>
       </c>
@@ -5834,7 +5883,7 @@
       <c r="G13" s="20"/>
       <c r="H13" s="17"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="s">
         <v>64</v>
       </c>
@@ -5850,7 +5899,7 @@
       <c r="G14" s="20"/>
       <c r="H14" s="17"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A15" s="5" t="s">
         <v>65</v>
       </c>
@@ -5866,7 +5915,7 @@
       <c r="G15" s="20"/>
       <c r="H15" s="17"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A16" s="5" t="s">
         <v>66</v>
       </c>
@@ -5882,7 +5931,7 @@
       <c r="G16" s="20"/>
       <c r="H16" s="17"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A17" s="5" t="s">
         <v>67</v>
       </c>
@@ -5898,7 +5947,7 @@
       <c r="G17" s="20"/>
       <c r="H17" s="17"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A18" s="5" t="s">
         <v>68</v>
       </c>
@@ -5914,7 +5963,7 @@
       <c r="G18" s="20"/>
       <c r="H18" s="17"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A19" s="5" t="s">
         <v>69</v>
       </c>
@@ -5930,7 +5979,7 @@
       <c r="G19" s="20"/>
       <c r="H19" s="17"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A20" s="5" t="s">
         <v>70</v>
       </c>
@@ -5946,7 +5995,7 @@
       <c r="G20" s="20"/>
       <c r="H20" s="17"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="12" x14ac:dyDescent="0.15">
       <c r="A21" s="5" t="s">
         <v>71</v>
       </c>
@@ -5962,7 +6011,7 @@
       <c r="G21" s="20"/>
       <c r="H21" s="17"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
       <c r="E22" s="17"/>
@@ -5970,7 +6019,7 @@
       <c r="G22" s="20"/>
       <c r="H22" s="17"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
@@ -5978,7 +6027,7 @@
       <c r="G23" s="20"/>
       <c r="H23" s="17"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
       <c r="E24" s="17"/>
@@ -5986,7 +6035,7 @@
       <c r="G24" s="20"/>
       <c r="H24" s="17"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
       <c r="E25" s="17"/>
@@ -5994,7 +6043,7 @@
       <c r="G25" s="20"/>
       <c r="H25" s="17"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C26" s="17"/>
       <c r="D26" s="17"/>
       <c r="E26" s="17"/>
@@ -6002,7 +6051,7 @@
       <c r="G26" s="20"/>
       <c r="H26" s="17"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
       <c r="E27" s="17"/>
@@ -6010,7 +6059,7 @@
       <c r="G27" s="20"/>
       <c r="H27" s="17"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
       <c r="E28" s="17"/>
@@ -6018,7 +6067,7 @@
       <c r="G28" s="20"/>
       <c r="H28" s="17"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
       <c r="E29" s="17"/>
@@ -6026,7 +6075,7 @@
       <c r="G29" s="20"/>
       <c r="H29" s="17"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
       <c r="E30" s="17"/>
@@ -6034,7 +6083,7 @@
       <c r="G30" s="20"/>
       <c r="H30" s="17"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C31" s="17"/>
       <c r="D31" s="17"/>
       <c r="E31" s="17"/>
@@ -6042,7 +6091,7 @@
       <c r="G31" s="20"/>
       <c r="H31" s="17"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C32" s="17"/>
       <c r="D32" s="17"/>
       <c r="E32" s="17"/>
@@ -6050,7 +6099,7 @@
       <c r="G32" s="20"/>
       <c r="H32" s="17"/>
     </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:8" x14ac:dyDescent="0.15">
       <c r="C33" s="17"/>
       <c r="D33" s="17"/>
       <c r="E33" s="17"/>
@@ -6058,7 +6107,7 @@
       <c r="G33" s="20"/>
       <c r="H33" s="17"/>
     </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:8" x14ac:dyDescent="0.15">
       <c r="C34" s="17"/>
       <c r="D34" s="17"/>
       <c r="E34" s="17"/>
@@ -6066,7 +6115,7 @@
       <c r="G34" s="20"/>
       <c r="H34" s="17"/>
     </row>
-    <row r="35" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:8" x14ac:dyDescent="0.15">
       <c r="C35" s="17"/>
       <c r="D35" s="17"/>
       <c r="E35" s="17"/>
@@ -6074,7 +6123,7 @@
       <c r="G35" s="20"/>
       <c r="H35" s="17"/>
     </row>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:8" x14ac:dyDescent="0.15">
       <c r="C36" s="17"/>
       <c r="D36" s="17"/>
       <c r="E36" s="17"/>
@@ -6082,7 +6131,7 @@
       <c r="G36" s="20"/>
       <c r="H36" s="17"/>
     </row>
-    <row r="37" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:8" x14ac:dyDescent="0.15">
       <c r="C37" s="17"/>
       <c r="D37" s="17"/>
       <c r="E37" s="17"/>
@@ -6090,7 +6139,7 @@
       <c r="G37" s="20"/>
       <c r="H37" s="17"/>
     </row>
-    <row r="38" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:8" x14ac:dyDescent="0.15">
       <c r="C38" s="17"/>
       <c r="D38" s="17"/>
       <c r="E38" s="17"/>
@@ -6098,7 +6147,7 @@
       <c r="G38" s="20"/>
       <c r="H38" s="17"/>
     </row>
-    <row r="39" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:8" x14ac:dyDescent="0.15">
       <c r="C39" s="17"/>
       <c r="D39" s="17"/>
       <c r="E39" s="17"/>
@@ -6106,7 +6155,7 @@
       <c r="G39" s="20"/>
       <c r="H39" s="17"/>
     </row>
-    <row r="40" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:8" x14ac:dyDescent="0.15">
       <c r="C40" s="17"/>
       <c r="D40" s="17"/>
       <c r="E40" s="17"/>
@@ -6114,7 +6163,7 @@
       <c r="G40" s="20"/>
       <c r="H40" s="17"/>
     </row>
-    <row r="41" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:8" x14ac:dyDescent="0.15">
       <c r="C41" s="17"/>
       <c r="D41" s="17"/>
       <c r="E41" s="17"/>
@@ -6122,7 +6171,7 @@
       <c r="G41" s="20"/>
       <c r="H41" s="17"/>
     </row>
-    <row r="42" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:8" x14ac:dyDescent="0.15">
       <c r="C42" s="17"/>
       <c r="D42" s="17"/>
       <c r="E42" s="17"/>
@@ -6130,7 +6179,7 @@
       <c r="G42" s="20"/>
       <c r="H42" s="17"/>
     </row>
-    <row r="43" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:8" x14ac:dyDescent="0.15">
       <c r="C43" s="17"/>
       <c r="D43" s="17"/>
       <c r="E43" s="17"/>
@@ -6138,7 +6187,7 @@
       <c r="G43" s="20"/>
       <c r="H43" s="17"/>
     </row>
-    <row r="44" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:8" x14ac:dyDescent="0.15">
       <c r="C44" s="17"/>
       <c r="D44" s="17"/>
       <c r="E44" s="17"/>
@@ -6146,7 +6195,7 @@
       <c r="G44" s="20"/>
       <c r="H44" s="17"/>
     </row>
-    <row r="45" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="3:8" x14ac:dyDescent="0.15">
       <c r="C45" s="17"/>
       <c r="D45" s="17"/>
       <c r="E45" s="17"/>
@@ -6154,7 +6203,7 @@
       <c r="G45" s="20"/>
       <c r="H45" s="17"/>
     </row>
-    <row r="46" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="3:8" x14ac:dyDescent="0.15">
       <c r="C46" s="17"/>
       <c r="D46" s="17"/>
       <c r="E46" s="17"/>
@@ -6162,7 +6211,7 @@
       <c r="G46" s="20"/>
       <c r="H46" s="17"/>
     </row>
-    <row r="47" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="3:8" x14ac:dyDescent="0.15">
       <c r="C47" s="17"/>
       <c r="D47" s="17"/>
       <c r="E47" s="17"/>
@@ -6170,7 +6219,7 @@
       <c r="G47" s="20"/>
       <c r="H47" s="17"/>
     </row>
-    <row r="48" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="3:8" x14ac:dyDescent="0.15">
       <c r="C48" s="17"/>
       <c r="D48" s="17"/>
       <c r="E48" s="17"/>
@@ -6184,26 +6233,26 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="4" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="4" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="4"/>
+    <col min="10" max="16384" width="9.1640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
         <v>47</v>
       </c>
@@ -6232,7 +6281,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="str">
         <f>VLOOKUP(B2,geo_cw!A$2:H$49,2)</f>
         <v>Mombasa</v>
@@ -6262,7 +6311,7 @@
         <v>78.2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="str">
         <f>VLOOKUP(B3,geo_cw!A$2:H$49,2)</f>
         <v>Kwale</v>
@@ -6292,7 +6341,7 @@
         <v>48.1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="str">
         <f>VLOOKUP(B4,geo_cw!A$2:H$49,2)</f>
         <v>Kilifi</v>
@@ -6322,7 +6371,7 @@
         <v>61.2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="str">
         <f>VLOOKUP(B5,geo_cw!A$2:H$49,2)</f>
         <v>Tana River</v>
@@ -6352,7 +6401,7 @@
         <v>36.799999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="str">
         <f>VLOOKUP(B6,geo_cw!A$2:H$49,2)</f>
         <v>Lamu</v>
@@ -6382,7 +6431,7 @@
         <v>56.2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="str">
         <f>VLOOKUP(B7,geo_cw!A$2:H$49,2)</f>
         <v>Taita Taveta</v>
@@ -6412,7 +6461,7 @@
         <v>50.4</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="str">
         <f>VLOOKUP(B8,geo_cw!A$2:H$49,2)</f>
         <v>Garissa</v>
@@ -6442,7 +6491,7 @@
         <v>30.4</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="str">
         <f>VLOOKUP(B9,geo_cw!A$2:H$49,2)</f>
         <v>Wajir</v>
@@ -6472,7 +6521,7 @@
         <v>10.7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="str">
         <f>VLOOKUP(B10,geo_cw!A$2:H$49,2)</f>
         <v>Mandera</v>
@@ -6502,7 +6551,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="str">
         <f>VLOOKUP(B11,geo_cw!A$2:H$49,2)</f>
         <v>Marsabit</v>
@@ -6532,7 +6581,7 @@
         <v>30.9</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="str">
         <f>VLOOKUP(B12,geo_cw!A$2:H$49,2)</f>
         <v>Isiolo</v>
@@ -6562,7 +6611,7 @@
         <v>43.9</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="str">
         <f>VLOOKUP(B13,geo_cw!A$2:H$49,2)</f>
         <v>Meru</v>
@@ -6592,7 +6641,7 @@
         <v>52.5</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="24" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="str">
         <f>VLOOKUP(B14,geo_cw!A$2:H$49,2)</f>
         <v>Tharaka-Nithi</v>
@@ -6622,7 +6671,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="str">
         <f>VLOOKUP(B15,geo_cw!A$2:H$49,2)</f>
         <v>Embu</v>
@@ -6652,7 +6701,7 @@
         <v>50.7</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="str">
         <f>VLOOKUP(B16,geo_cw!A$2:H$49,2)</f>
         <v>Kitui</v>
@@ -6682,7 +6731,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="str">
         <f>VLOOKUP(B17,geo_cw!A$2:H$49,2)</f>
         <v>Machakos</v>
@@ -6712,7 +6761,7 @@
         <v>63.6</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="str">
         <f>VLOOKUP(B18,geo_cw!A$2:H$49,2)</f>
         <v>Makueni</v>
@@ -6742,7 +6791,7 @@
         <v>40.799999999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="str">
         <f>VLOOKUP(B19,geo_cw!A$2:H$49,2)</f>
         <v>Nyandarua</v>
@@ -6772,7 +6821,7 @@
         <v>46.5</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="str">
         <f>VLOOKUP(B20,geo_cw!A$2:H$49,2)</f>
         <v>Nyeri</v>
@@ -6802,7 +6851,7 @@
         <v>66.7</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="str">
         <f>VLOOKUP(B21,geo_cw!A$2:H$49,2)</f>
         <v>Kirinyaga</v>
@@ -6832,7 +6881,7 @@
         <v>51.6</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="str">
         <f>VLOOKUP(B22,geo_cw!A$2:H$49,2)</f>
         <v>Murang'a</v>
@@ -6862,7 +6911,7 @@
         <v>41.7</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="str">
         <f>VLOOKUP(B23,geo_cw!A$2:H$49,2)</f>
         <v>Kiambu</v>
@@ -6892,7 +6941,7 @@
         <v>67.599999999999994</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="str">
         <f>VLOOKUP(B24,geo_cw!A$2:H$49,2)</f>
         <v>Turkana</v>
@@ -6922,7 +6971,7 @@
         <v>54.9</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="str">
         <f>VLOOKUP(B25,geo_cw!A$2:H$49,2)</f>
         <v>West Pokot</v>
@@ -6952,7 +7001,7 @@
         <v>19.3</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="str">
         <f>VLOOKUP(B26,geo_cw!A$2:H$49,2)</f>
         <v>Samburu</v>
@@ -6982,7 +7031,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="str">
         <f>VLOOKUP(B27,geo_cw!A$2:H$49,2)</f>
         <v>Trans Nzoia</v>
@@ -7012,7 +7061,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="str">
         <f>VLOOKUP(B28,geo_cw!A$2:H$49,2)</f>
         <v>Uasin Gishu</v>
@@ -7042,10 +7091,9 @@
         <v>51.5</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="str">
-        <f>VLOOKUP(B29,geo_cw!A$2:H$49,2)</f>
-        <v>Busia</v>
+    <row r="29" spans="1:9" ht="24" x14ac:dyDescent="0.15">
+      <c r="A29" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>27</v>
@@ -7072,7 +7120,7 @@
         <v>26.7</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="str">
         <f>VLOOKUP(B30,geo_cw!A$2:H$49,2)</f>
         <v>Nandi</v>
@@ -7102,7 +7150,7 @@
         <v>24.8</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="str">
         <f>VLOOKUP(B31,geo_cw!A$2:H$49,2)</f>
         <v>Baringo</v>
@@ -7132,7 +7180,7 @@
         <v>49.8</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="str">
         <f>VLOOKUP(B32,geo_cw!A$2:H$49,2)</f>
         <v>Laikipia</v>
@@ -7162,7 +7210,7 @@
         <v>48.9</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="str">
         <f>VLOOKUP(B33,geo_cw!A$2:H$49,2)</f>
         <v>Nakuru</v>
@@ -7192,7 +7240,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="str">
         <f>VLOOKUP(B34,geo_cw!A$2:H$49,2)</f>
         <v>Narok</v>
@@ -7222,7 +7270,7 @@
         <v>59.6</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A35" s="4" t="str">
         <f>VLOOKUP(B35,geo_cw!A$2:H$49,2)</f>
         <v>Kajiado</v>
@@ -7252,7 +7300,7 @@
         <v>63.4</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A36" s="4" t="str">
         <f>VLOOKUP(B36,geo_cw!A$2:H$49,2)</f>
         <v>Kericho</v>
@@ -7282,7 +7330,7 @@
         <v>34.5</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="str">
         <f>VLOOKUP(B37,geo_cw!A$2:H$49,2)</f>
         <v>Bomet</v>
@@ -7312,7 +7360,7 @@
         <v>19.899999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="str">
         <f>VLOOKUP(B38,geo_cw!A$2:H$49,2)</f>
         <v>Kakamega</v>
@@ -7342,7 +7390,7 @@
         <v>27.4</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="str">
         <f>VLOOKUP(B39,geo_cw!A$2:H$49,2)</f>
         <v>Vihiga</v>
@@ -7372,7 +7420,7 @@
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="str">
         <f>VLOOKUP(B40,geo_cw!A$2:H$49,2)</f>
         <v>Bungoma</v>
@@ -7402,7 +7450,7 @@
         <v>38.299999999999997</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A41" s="4" t="str">
         <f>VLOOKUP(B41,geo_cw!A$2:H$49,2)</f>
         <v>Busia</v>
@@ -7432,7 +7480,7 @@
         <v>21.8</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A42" s="4" t="str">
         <f>VLOOKUP(B42,geo_cw!A$2:H$49,2)</f>
         <v>Siaya</v>
@@ -7462,7 +7510,7 @@
         <v>37.799999999999997</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A43" s="4" t="str">
         <f>VLOOKUP(B43,geo_cw!A$2:H$49,2)</f>
         <v>Kisumu</v>
@@ -7492,7 +7540,7 @@
         <v>54.2</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A44" s="4" t="str">
         <f>VLOOKUP(B44,geo_cw!A$2:H$49,2)</f>
         <v>Homa Bay</v>
@@ -7522,7 +7570,7 @@
         <v>30.7</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A45" s="4" t="str">
         <f>VLOOKUP(B45,geo_cw!A$2:H$49,2)</f>
         <v>Migori</v>
@@ -7552,7 +7600,7 @@
         <v>27.2</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A46" s="4" t="str">
         <f>VLOOKUP(B46,geo_cw!A$2:H$49,2)</f>
         <v>Kisii</v>
@@ -7582,7 +7630,7 @@
         <v>29.3</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A47" s="4" t="str">
         <f>VLOOKUP(B47,geo_cw!A$2:H$49,2)</f>
         <v>Nyamira</v>
@@ -7612,7 +7660,7 @@
         <v>38.700000000000003</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A48" s="4" t="str">
         <f>VLOOKUP(B48,geo_cw!A$2:H$49,2)</f>
         <v>Nairobi</v>
@@ -7642,7 +7690,10 @@
         <v>86.4</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" ht="12" x14ac:dyDescent="0.15">
+      <c r="A49" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="B49" s="9" t="s">
         <v>84</v>
       </c>
@@ -7674,31 +7725,31 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="4" customWidth="1"/>
     <col min="2" max="2" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="4"/>
+    <col min="3" max="3" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.1640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>47</v>
       </c>
@@ -7736,7 +7787,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="str">
         <f>VLOOKUP(B2,geo_cw!A$2:H$49,2)</f>
         <v>Mombasa</v>
@@ -7775,7 +7826,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="str">
         <f>VLOOKUP(B3,geo_cw!A$2:H$49,2)</f>
         <v>Kwale</v>
@@ -7814,7 +7865,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="str">
         <f>VLOOKUP(B4,geo_cw!A$2:H$49,2)</f>
         <v>Kilifi</v>
@@ -7853,7 +7904,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="str">
         <f>VLOOKUP(B5,geo_cw!A$2:H$49,2)</f>
         <v>Tana River</v>
@@ -7892,7 +7943,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="str">
         <f>VLOOKUP(B6,geo_cw!A$2:H$49,2)</f>
         <v>Lamu</v>
@@ -7931,7 +7982,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="str">
         <f>VLOOKUP(B7,geo_cw!A$2:H$49,2)</f>
         <v>Taita Taveta</v>
@@ -7970,7 +8021,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="str">
         <f>VLOOKUP(B8,geo_cw!A$2:H$49,2)</f>
         <v>Garissa</v>
@@ -8009,7 +8060,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="str">
         <f>VLOOKUP(B9,geo_cw!A$2:H$49,2)</f>
         <v>Wajir</v>
@@ -8048,7 +8099,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="str">
         <f>VLOOKUP(B10,geo_cw!A$2:H$49,2)</f>
         <v>Mandera</v>
@@ -8087,7 +8138,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="str">
         <f>VLOOKUP(B11,geo_cw!A$2:H$49,2)</f>
         <v>Marsabit</v>
@@ -8126,7 +8177,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="str">
         <f>VLOOKUP(B12,geo_cw!A$2:H$49,2)</f>
         <v>Isiolo</v>
@@ -8165,7 +8216,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="str">
         <f>VLOOKUP(B13,geo_cw!A$2:H$49,2)</f>
         <v>Meru</v>
@@ -8204,7 +8255,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="24" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="str">
         <f>VLOOKUP(B14,geo_cw!A$2:H$49,2)</f>
         <v>Tharaka-Nithi</v>
@@ -8243,7 +8294,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="str">
         <f>VLOOKUP(B15,geo_cw!A$2:H$49,2)</f>
         <v>Embu</v>
@@ -8282,7 +8333,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="str">
         <f>VLOOKUP(B16,geo_cw!A$2:H$49,2)</f>
         <v>Kitui</v>
@@ -8321,7 +8372,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="str">
         <f>VLOOKUP(B17,geo_cw!A$2:H$49,2)</f>
         <v>Machakos</v>
@@ -8360,7 +8411,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="str">
         <f>VLOOKUP(B18,geo_cw!A$2:H$49,2)</f>
         <v>Makueni</v>
@@ -8399,7 +8450,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="str">
         <f>VLOOKUP(B19,geo_cw!A$2:H$49,2)</f>
         <v>Nyandarua</v>
@@ -8438,7 +8489,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="str">
         <f>VLOOKUP(B20,geo_cw!A$2:H$49,2)</f>
         <v>Nyeri</v>
@@ -8477,7 +8528,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="str">
         <f>VLOOKUP(B21,geo_cw!A$2:H$49,2)</f>
         <v>Kirinyaga</v>
@@ -8516,7 +8567,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="str">
         <f>VLOOKUP(B22,geo_cw!A$2:H$49,2)</f>
         <v>Murang'a</v>
@@ -8555,7 +8606,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="str">
         <f>VLOOKUP(B23,geo_cw!A$2:H$49,2)</f>
         <v>Kiambu</v>
@@ -8594,7 +8645,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="str">
         <f>VLOOKUP(B24,geo_cw!A$2:H$49,2)</f>
         <v>Turkana</v>
@@ -8633,7 +8684,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="str">
         <f>VLOOKUP(B25,geo_cw!A$2:H$49,2)</f>
         <v>West Pokot</v>
@@ -8672,7 +8723,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="str">
         <f>VLOOKUP(B26,geo_cw!A$2:H$49,2)</f>
         <v>Samburu</v>
@@ -8711,7 +8762,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="str">
         <f>VLOOKUP(B27,geo_cw!A$2:H$49,2)</f>
         <v>Trans Nzoia</v>
@@ -8750,7 +8801,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="str">
         <f>VLOOKUP(B28,geo_cw!A$2:H$49,2)</f>
         <v>Uasin Gishu</v>
@@ -8789,10 +8840,9 @@
         <v>535</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="str">
-        <f>VLOOKUP(B29,geo_cw!A$2:H$49,2)</f>
-        <v>Busia</v>
+    <row r="29" spans="1:12" ht="24" x14ac:dyDescent="0.15">
+      <c r="A29" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>27</v>
@@ -8828,7 +8878,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="str">
         <f>VLOOKUP(B30,geo_cw!A$2:H$49,2)</f>
         <v>Nandi</v>
@@ -8867,7 +8917,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="str">
         <f>VLOOKUP(B31,geo_cw!A$2:H$49,2)</f>
         <v>Baringo</v>
@@ -8906,7 +8956,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="str">
         <f>VLOOKUP(B32,geo_cw!A$2:H$49,2)</f>
         <v>Laikipia</v>
@@ -8945,7 +8995,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="str">
         <f>VLOOKUP(B33,geo_cw!A$2:H$49,2)</f>
         <v>Nakuru</v>
@@ -8984,7 +9034,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="str">
         <f>VLOOKUP(B34,geo_cw!A$2:H$49,2)</f>
         <v>Narok</v>
@@ -9023,7 +9073,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A35" s="4" t="str">
         <f>VLOOKUP(B35,geo_cw!A$2:H$49,2)</f>
         <v>Kajiado</v>
@@ -9062,7 +9112,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A36" s="4" t="str">
         <f>VLOOKUP(B36,geo_cw!A$2:H$49,2)</f>
         <v>Kericho</v>
@@ -9101,7 +9151,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="str">
         <f>VLOOKUP(B37,geo_cw!A$2:H$49,2)</f>
         <v>Bomet</v>
@@ -9140,7 +9190,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="str">
         <f>VLOOKUP(B38,geo_cw!A$2:H$49,2)</f>
         <v>Kakamega</v>
@@ -9179,7 +9229,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="str">
         <f>VLOOKUP(B39,geo_cw!A$2:H$49,2)</f>
         <v>Vihiga</v>
@@ -9218,7 +9268,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="str">
         <f>VLOOKUP(B40,geo_cw!A$2:H$49,2)</f>
         <v>Bungoma</v>
@@ -9257,7 +9307,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A41" s="4" t="str">
         <f>VLOOKUP(B41,geo_cw!A$2:H$49,2)</f>
         <v>Busia</v>
@@ -9296,7 +9346,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A42" s="4" t="str">
         <f>VLOOKUP(B42,geo_cw!A$2:H$49,2)</f>
         <v>Siaya</v>
@@ -9335,7 +9385,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A43" s="4" t="str">
         <f>VLOOKUP(B43,geo_cw!A$2:H$49,2)</f>
         <v>Kisumu</v>
@@ -9374,7 +9424,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A44" s="4" t="str">
         <f>VLOOKUP(B44,geo_cw!A$2:H$49,2)</f>
         <v>Homa Bay</v>
@@ -9413,7 +9463,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A45" s="4" t="str">
         <f>VLOOKUP(B45,geo_cw!A$2:H$49,2)</f>
         <v>Migori</v>
@@ -9452,7 +9502,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A46" s="4" t="str">
         <f>VLOOKUP(B46,geo_cw!A$2:H$49,2)</f>
         <v>Kisii</v>
@@ -9491,7 +9541,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A47" s="4" t="str">
         <f>VLOOKUP(B47,geo_cw!A$2:H$49,2)</f>
         <v>Nyamira</v>
@@ -9530,7 +9580,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A48" s="4" t="str">
         <f>VLOOKUP(B48,geo_cw!A$2:H$49,2)</f>
         <v>Nairobi</v>
@@ -9569,7 +9619,10 @@
         <v>1582</v>
       </c>
     </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A49" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="B49" s="4" t="s">
         <v>84</v>
       </c>
@@ -9610,22 +9663,22 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="11" width="9.140625" style="25"/>
-    <col min="12" max="12" width="12.42578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="25"/>
+    <col min="1" max="1" width="12.6640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="11" width="9.1640625" style="25"/>
+    <col min="12" max="12" width="12.5" style="25" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.1640625" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>47</v>
       </c>
@@ -9663,7 +9716,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="str">
         <f>VLOOKUP(B2,geo_cw!A$2:H$49,2)</f>
         <v>Mombasa</v>
@@ -9702,7 +9755,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="str">
         <f>VLOOKUP(B3,geo_cw!A$2:H$49,2)</f>
         <v>Kwale</v>
@@ -9741,7 +9794,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="str">
         <f>VLOOKUP(B4,geo_cw!A$2:H$49,2)</f>
         <v>Kilifi</v>
@@ -9780,7 +9833,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="str">
         <f>VLOOKUP(B5,geo_cw!A$2:H$49,2)</f>
         <v>Tana River</v>
@@ -9819,7 +9872,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="str">
         <f>VLOOKUP(B6,geo_cw!A$2:H$49,2)</f>
         <v>Lamu</v>
@@ -9858,7 +9911,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="str">
         <f>VLOOKUP(B7,geo_cw!A$2:H$49,2)</f>
         <v>Taita Taveta</v>
@@ -9897,7 +9950,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="str">
         <f>VLOOKUP(B8,geo_cw!A$2:H$49,2)</f>
         <v>Garissa</v>
@@ -9936,7 +9989,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="str">
         <f>VLOOKUP(B9,geo_cw!A$2:H$49,2)</f>
         <v>Wajir</v>
@@ -9975,7 +10028,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="str">
         <f>VLOOKUP(B10,geo_cw!A$2:H$49,2)</f>
         <v>Mandera</v>
@@ -10014,7 +10067,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="str">
         <f>VLOOKUP(B11,geo_cw!A$2:H$49,2)</f>
         <v>Marsabit</v>
@@ -10053,7 +10106,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="str">
         <f>VLOOKUP(B12,geo_cw!A$2:H$49,2)</f>
         <v>Isiolo</v>
@@ -10092,7 +10145,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="str">
         <f>VLOOKUP(B13,geo_cw!A$2:H$49,2)</f>
         <v>Meru</v>
@@ -10131,7 +10184,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="24" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="str">
         <f>VLOOKUP(B14,geo_cw!A$2:H$49,2)</f>
         <v>Tharaka-Nithi</v>
@@ -10170,7 +10223,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="str">
         <f>VLOOKUP(B15,geo_cw!A$2:H$49,2)</f>
         <v>Embu</v>
@@ -10209,7 +10262,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="str">
         <f>VLOOKUP(B16,geo_cw!A$2:H$49,2)</f>
         <v>Kitui</v>
@@ -10248,7 +10301,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="str">
         <f>VLOOKUP(B17,geo_cw!A$2:H$49,2)</f>
         <v>Machakos</v>
@@ -10287,7 +10340,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="str">
         <f>VLOOKUP(B18,geo_cw!A$2:H$49,2)</f>
         <v>Makueni</v>
@@ -10326,7 +10379,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="str">
         <f>VLOOKUP(B19,geo_cw!A$2:H$49,2)</f>
         <v>Nyandarua</v>
@@ -10365,7 +10418,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="str">
         <f>VLOOKUP(B20,geo_cw!A$2:H$49,2)</f>
         <v>Nyeri</v>
@@ -10404,7 +10457,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="str">
         <f>VLOOKUP(B21,geo_cw!A$2:H$49,2)</f>
         <v>Kirinyaga</v>
@@ -10443,7 +10496,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="str">
         <f>VLOOKUP(B22,geo_cw!A$2:H$49,2)</f>
         <v>Murang'a</v>
@@ -10482,7 +10535,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="str">
         <f>VLOOKUP(B23,geo_cw!A$2:H$49,2)</f>
         <v>Kiambu</v>
@@ -10521,7 +10574,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="str">
         <f>VLOOKUP(B24,geo_cw!A$2:H$49,2)</f>
         <v>Turkana</v>
@@ -10560,7 +10613,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="str">
         <f>VLOOKUP(B25,geo_cw!A$2:H$49,2)</f>
         <v>West Pokot</v>
@@ -10599,7 +10652,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="str">
         <f>VLOOKUP(B26,geo_cw!A$2:H$49,2)</f>
         <v>Samburu</v>
@@ -10638,7 +10691,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="str">
         <f>VLOOKUP(B27,geo_cw!A$2:H$49,2)</f>
         <v>Trans Nzoia</v>
@@ -10677,7 +10730,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="str">
         <f>VLOOKUP(B28,geo_cw!A$2:H$49,2)</f>
         <v>Uasin Gishu</v>
@@ -10716,7 +10769,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" ht="24" x14ac:dyDescent="0.15">
       <c r="A29" s="4" t="str">
         <f>VLOOKUP(B29,geo_cw!A$2:H$49,2)</f>
         <v>Elgeyo-Marakwet</v>
@@ -10755,7 +10808,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="str">
         <f>VLOOKUP(B30,geo_cw!A$2:H$49,2)</f>
         <v>Nandi</v>
@@ -10794,7 +10847,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="str">
         <f>VLOOKUP(B31,geo_cw!A$2:H$49,2)</f>
         <v>Baringo</v>
@@ -10833,7 +10886,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="str">
         <f>VLOOKUP(B32,geo_cw!A$2:H$49,2)</f>
         <v>Laikipia</v>
@@ -10872,7 +10925,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="str">
         <f>VLOOKUP(B33,geo_cw!A$2:H$49,2)</f>
         <v>Nakuru</v>
@@ -10911,7 +10964,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="str">
         <f>VLOOKUP(B34,geo_cw!A$2:H$49,2)</f>
         <v>Narok</v>
@@ -10950,7 +11003,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A35" s="4" t="str">
         <f>VLOOKUP(B35,geo_cw!A$2:H$49,2)</f>
         <v>Kajiado</v>
@@ -10989,7 +11042,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A36" s="4" t="str">
         <f>VLOOKUP(B36,geo_cw!A$2:H$49,2)</f>
         <v>Kericho</v>
@@ -11028,7 +11081,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="str">
         <f>VLOOKUP(B37,geo_cw!A$2:H$49,2)</f>
         <v>Bomet</v>
@@ -11067,7 +11120,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="str">
         <f>VLOOKUP(B38,geo_cw!A$2:H$49,2)</f>
         <v>Kakamega</v>
@@ -11106,7 +11159,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="str">
         <f>VLOOKUP(B39,geo_cw!A$2:H$49,2)</f>
         <v>Vihiga</v>
@@ -11145,7 +11198,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="str">
         <f>VLOOKUP(B40,geo_cw!A$2:H$49,2)</f>
         <v>Bungoma</v>
@@ -11184,7 +11237,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A41" s="4" t="str">
         <f>VLOOKUP(B41,geo_cw!A$2:H$49,2)</f>
         <v>Busia</v>
@@ -11223,7 +11276,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A42" s="4" t="str">
         <f>VLOOKUP(B42,geo_cw!A$2:H$49,2)</f>
         <v>Siaya</v>
@@ -11262,7 +11315,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A43" s="4" t="str">
         <f>VLOOKUP(B43,geo_cw!A$2:H$49,2)</f>
         <v>Kisumu</v>
@@ -11301,7 +11354,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A44" s="4" t="str">
         <f>VLOOKUP(B44,geo_cw!A$2:H$49,2)</f>
         <v>Homa Bay</v>
@@ -11340,7 +11393,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A45" s="4" t="str">
         <f>VLOOKUP(B45,geo_cw!A$2:H$49,2)</f>
         <v>Migori</v>
@@ -11379,7 +11432,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A46" s="4" t="str">
         <f>VLOOKUP(B46,geo_cw!A$2:H$49,2)</f>
         <v>Kisii</v>
@@ -11418,7 +11471,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A47" s="4" t="str">
         <f>VLOOKUP(B47,geo_cw!A$2:H$49,2)</f>
         <v>Nyamira</v>
@@ -11457,7 +11510,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A48" s="4" t="str">
         <f>VLOOKUP(B48,geo_cw!A$2:H$49,2)</f>
         <v>Nairobi</v>
@@ -11496,8 +11549,10 @@
         <v>1582</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A49" s="4"/>
+    <row r="49" spans="1:12" ht="12" x14ac:dyDescent="0.15">
+      <c r="A49" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="B49" s="9" t="s">
         <v>84</v>
       </c>
@@ -11538,20 +11593,20 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L38" sqref="L38"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>48</v>
       </c>
@@ -11577,7 +11632,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
@@ -11603,7 +11658,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>35</v>
       </c>
@@ -11629,7 +11684,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>38</v>
       </c>
@@ -11655,7 +11710,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>39</v>
       </c>
@@ -11681,7 +11736,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>95</v>
       </c>
@@ -11707,7 +11762,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -11733,7 +11788,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -11759,7 +11814,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>42</v>
       </c>
@@ -11785,7 +11840,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -11811,7 +11866,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>33</v>
       </c>
@@ -11837,7 +11892,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>36</v>
       </c>
@@ -11863,7 +11918,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>34</v>
       </c>
@@ -11889,7 +11944,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
@@ -11915,7 +11970,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>2</v>
       </c>
@@ -11941,7 +11996,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
@@ -11967,7 +12022,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>44</v>
       </c>
@@ -11993,7 +12048,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>41</v>
       </c>
@@ -12019,7 +12074,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
@@ -12045,7 +12100,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>1</v>
       </c>
@@ -12071,7 +12126,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>30</v>
       </c>
@@ -12097,7 +12152,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>4</v>
       </c>
@@ -12123,7 +12178,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>15</v>
       </c>
@@ -12149,7 +12204,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>16</v>
       </c>
@@ -12175,7 +12230,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>8</v>
       </c>
@@ -12201,7 +12256,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>9</v>
       </c>
@@ -12227,7 +12282,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>11</v>
       </c>
@@ -12253,7 +12308,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>43</v>
       </c>
@@ -12279,7 +12334,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>0</v>
       </c>
@@ -12305,7 +12360,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>62</v>
       </c>
@@ -12331,7 +12386,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>46</v>
       </c>
@@ -12357,7 +12412,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
@@ -12383,7 +12438,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>28</v>
       </c>
@@ -12409,7 +12464,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
@@ -12435,7 +12490,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>84</v>
       </c>
@@ -12449,7 +12504,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>45</v>
       </c>
@@ -12475,7 +12530,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>17</v>
       </c>
@@ -12501,7 +12556,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>18</v>
       </c>
@@ -12527,7 +12582,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>24</v>
       </c>
@@ -12553,7 +12608,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>40</v>
       </c>
@@ -12579,7 +12634,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>60</v>
       </c>
@@ -12605,7 +12660,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>3</v>
       </c>
@@ -12631,7 +12686,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>61</v>
       </c>
@@ -12657,7 +12712,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>25</v>
       </c>
@@ -12683,7 +12738,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>22</v>
       </c>
@@ -12709,7 +12764,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>26</v>
       </c>
@@ -12735,7 +12790,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>37</v>
       </c>
@@ -12761,7 +12816,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>7</v>
       </c>
@@ -12787,7 +12842,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>23</v>
       </c>

</xml_diff>